<commit_message>
Removed Some Unwanted Workflow to Keep it Simple
</commit_message>
<xml_diff>
--- a/Data/Output/result.xlsx
+++ b/Data/Output/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satish\OneDrive\Documents\UiPath\Compare-Different-UiPath-OCR-Engines\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7F2FC7-D2BE-4211-93D6-3EE8795B5517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA06169F-C8CA-4AF7-8664-62DC72F10469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{16592C77-DD30-477E-B54F-FB0FEC03AAAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68962825-7541-4C28-91E9-1543C78B71D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Microsoft</t>
   </si>
@@ -68,171 +68,6 @@
 9400m_x000D_
 -$100.00_x000D_
 $500.00</t>
-  </si>
-  <si>
-    <t>Data\Input\02-Short-stories.pdf</t>
-  </si>
-  <si>
-    <t>Gift Of the Magi_x000D_
-ONE DOLLAR AND EIGHTY-SEVEN cp.vrs. That was all. And sixty_x000D_
-cents of it was in pennies. pennies saved one and two at a time by_x000D_
-bulldozing the grcx•cr and the vegetable man and the butcher_x000D_
-until one's cheek burned with the silent imputation of parsimony_x000D_
-that such dealing implied. Three times Della counted it._x000D_
-One dollar and eighty—seven Cents. And the next day would be_x000D_
-Christma s._x000D_
-There uas clearly nothing left to do but flop dou•n on the_x000D_
-shabby little couch and howl. So Della did it. Which instigates the_x000D_
-moral reflection that life is made up Of sobs, sniffles, and smiles,_x000D_
-with sniffles predominating._x000D_
-VVhiIe the mistress of the home is gradually subsiding from the_x000D_
-first stage to the second, take a 100k at the home. A furnished flat_x000D_
-at $8 per week. It did not exactly Irggar description, but it cer-_x000D_
-tainly had that word on the lcnjk•out for the mendicancy squad._x000D_
-In the vestibule Was a into Which no letter_x000D_
-would go, and an electric button from which no mortal finger_x000D_
-cuuld coax a ring. Also aplYrtaining thereunto was a card bearing_x000D_
-the name 'Mr. James Dillingham Young.'_x000D_
-The 'Dillingham' had been flung to the breeze during a former_x000D_
-Of prosperity when its Eumssessor was being paid SS()_x000D_
-week. Now, when incorne was shrunk to $20, the letters of_x000D_
-looked blurred, as though they Were thinking seri-_x000D_
-ously of contracting to a modest and unassuming D. But whenever_x000D_
-Mr. James Dillingham Young came home and reached his flat_x000D_
-above he was called "Jim' and greatly hugged by Mrs. James_x000D_
-Dillingham Young, already introduced to you as Della. Which is_x000D_
-all very_x000D_
-Della finished her cry and attended to her cheeks with the_x000D_
-rag. She by the Window and out dully at a_x000D_
-grey eat walking a grey fence in a grey backyard. To-morrow_x000D_
-would be Christmas Day, and she had only $1.87 with which to_x000D_
-buy Jim a present. She had been saving every penny she could for</t>
-  </si>
-  <si>
-    <t>Data\Input\03-Invoice-sample.pdf</t>
-  </si>
-  <si>
-    <t>C gtirpd/nroirm_x000D_
-From:_x000D_
-DEMO - Sliced Invoices_x000D_
-suite SA.1204_x000D_
-123 Somewhere Street_x000D_
-Your City AZ 12345_x000D_
-admin Com_x000D_
-Test Business_x000D_
-123 Somewhere St_x000D_
-Melbourne. VIC 3000_x000D_
-test@test.com Invoice Number_x000D_
-Order Number_x000D_
-Invoice Date_x000D_
-Oue Oate_x000D_
-Total Due_x000D_
-RaWPrice_x000D_
-Sas co Sub Total_x000D_
-Total Invoice_x000D_
-INV-3337_x000D_
-January 25, 2016_x000D_
-January 31 2016_x000D_
-Hrs/Qty_x000D_
-1.00_x000D_
-ANZ Bank Service_x000D_
-Web Design_x000D_
-This is a sample description... Adjust Sub Total_x000D_
-$85.00_x000D_
-ACCS 1234 1234_x000D_
-4321 432_x000D_
-Payment is due within 30 days from date of invoice. Late payment is subject to fees of per month._x000D_
-Thanks for choosing DEMO - Sliced Invoices admin@slicedinvoices.com_x000D_
-Page III</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Parker Tech_x000D_
-74 Lincoln Green Lane_x000D_
-Church Stoke, PA 19402_x000D_
-(123) 456-7890_x000D_
-' o_x000D_
-1_x000D_
-l we be_x000D_
-_ Submitted on 9/9/2016_x000D_
-Invoice for Payable to »- Invoice #-_x000D_
-Name Bobby John 12345_x000D_
-Company name Bobby Co. ~_x000D_
-Email bobby@john.com_x000D_
-Street address Project Due date_x000D_
-City, State, Zip Project name 9/16/2016_x000D_
-Description Qty Unit price Total price_x000D_
-Item #1 1 $20000 $200.00_x000D_
-Item #2 x ‘ 2 $20030 $400.00_x000D_
-$0.00_x000D_
-$0.00_x000D_
-Notes: Subtotal $600.00_x000D_
-Adjustments —$100.00</t>
-  </si>
-  <si>
-    <t>I_x000D_
-The Gift of the Magi_x000D_
-ONE DOLLAR AND EIGH'I'Y-SEVEN CENTS. That was all. And sixty_x000D_
-cents of it was in pennies. Pennies saved one and two at a time by_x000D_
-bulldozing the grocer and the vegetable man and the butcher_x000D_
-until one’s cheek burned with the silent imputation of parsimony_x000D_
-that such close dealing implied. Three times Della counted it._x000D_
-One dollar and eighty-seven cents. And the next day would be_x000D_
-Christmas._x000D_
-There was clearly nothing left to do but flop down on the_x000D_
-' shabby little couch and bowl. So Della did it. Which instigates the_x000D_
-moral reﬂection that life is made up of sobs, snifﬂes, and smiles,_x000D_
-with snifﬂes predominating._x000D_
-While the mistress of the home is gradually subsiding from the_x000D_
-ﬁrst stage to the second, take a look at the home. A furnished ﬂat_x000D_
-at $8 per week. It did not exactly beggar description, but it cer-_x000D_
-tainly had that word on the look-out for the mendicancy squad._x000D_
-In the vestibule below was a letter-box into which no letter_x000D_
-would go, and an electric button from which no mortal ﬁnger_x000D_
-could coax a ring. Also appertaining thereunto was a card bearing_x000D_
-the name ‘Mr. James Dillingham Young.’_x000D_
-The ‘Dillingham’ had been ﬂung to the breeze during a former_x000D_
-period of prosperity when its possessor was being paid $30 per_x000D_
-week. Now, when the income was shrunk to $20, the letters of_x000D_
-‘Dillingham’ looked blurred, as though they were thinking seri-_x000D_
-ously of contracting to a modest and unassuming D. But whenever_x000D_
-Mr. James Dillingham Young came home and reached his ﬂat_x000D_
-above he was called ‘Jim’ and greatly hugged by Mrs. James_x000D_
-Dillingham Young, already introduced to you as Della. Which is_x000D_
-all very good._x000D_
-Della ﬁnished her cry and attended to her cheeks with the_x000D_
-powder rag. She stood by the window and looked out dully at a_x000D_
-grey cat walking a grey fence in a grey backyard. To-morrow_x000D_
-would be Christmas Day, and she had only $1.87 with which to_x000D_
-buy Jim 3 present. She had been saving every penny she could for</t>
-  </si>
-  <si>
-    <t>Qgé’é'ced/xzi/oiceo_x000D_
-From I Invoice Number I le-3337 I_x000D_
-DEMO - Sliced Invoices I Order Number I 12345 I_x000D_
-Suite 5A-1204 I invoice Date I January 25, 2016 I_x000D_
-123 Somewhere Street I Due Date I January 31, 2016 I_x000D_
-Your City AZ 12345_x000D_
-admin@s|icedinvoices.com I Total Due I $9350 I_x000D_
-To:_x000D_
-Test Business_x000D_
-123 Somewhere St_x000D_
-Melbourne, VIC 3000 ,_x000D_
-test@test.com -_x000D_
-I Hrs/Qty I Service , I , I Rate/Price I Adjust I Sub Total I_x000D_
-Web Design , 77 7_x000D_
-I 1'00 I This is a sample description... I $8500 I (100% I $8500 I_x000D_
-I . Sub Total I $85.00 I_x000D_
-. ‘ ' I Tax I $8.50 I_x000D_
-I Total I $93.50 I_x000D_
-ANZ Bank_x000D_
-ACC # 1234 1234 ,_x000D_
-BSB # 4321 432 ._x000D_
-Payment is due within 30 days from date of invoice. Late payment is subject to fees of 5% per month._x000D_
-Thanks for choosing DEMO - Sliced Invoices l admin@s|icedinvoices.com_x000D_
-Page 1/1</t>
   </si>
   <si>
     <t>Microsoft Cloud</t>
@@ -281,6 +116,100 @@
 $500.00</t>
   </si>
   <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Parker Tech_x000D_
+74 Lincoln Green Lane_x000D_
+Church Stoke, PA 19402_x000D_
+(123) 456-7890_x000D_
+' o_x000D_
+1_x000D_
+l we be_x000D_
+_ Submitted on 9/9/2016_x000D_
+Invoice for Payable to »- Invoice #-_x000D_
+Name Bobby John 12345_x000D_
+Company name Bobby Co. ~_x000D_
+Email bobby@john.com_x000D_
+Street address Project Due date_x000D_
+City, State, Zip Project name 9/16/2016_x000D_
+Description Qty Unit price Total price_x000D_
+Item #1 1 $20000 $200.00_x000D_
+Item #2 x ‘ 2 $20030 $400.00_x000D_
+$0.00_x000D_
+$0.00_x000D_
+Notes: Subtotal $600.00_x000D_
+Adjustments —$100.00</t>
+  </si>
+  <si>
+    <t>Google Cloud</t>
+  </si>
+  <si>
+    <t>ABBYY Cloud</t>
+  </si>
+  <si>
+    <t>﻿Parker Tech_x000D_
+74 Lincoln Green Lane_x000D_
+Church Stoke, PA 19402_x000D_
+(123) 456-7890_x000D_
+Invoice_x000D_
+Submitted on 9/9/2016_x000D_
+Invoice for                   Payable to            Invoice #_x000D_
+Name                          Bobby John            12345_x000D_
+Company name                  Bobby Co._x000D_
+Email                         bobby@john.com_x000D_
+Street address                Project               Due date_x000D_
+City, State, Zip              Project name          9/16/2016_x000D_
+Description                                   Qty        Unit price           Total price_x000D_
+Item #1                                        1                   $200.00     $200.00_x000D_
+Item #2                                                                        $400.00_x000D_
+                                               2                   $200.00_x000D_
+                                                                                   $0.00_x000D_
+                                                                                   $0.00_x000D_
+Notes:                                                             Subtotal    $600.00_x000D_
+                                                     Adjustments -$100.00_x000D_
+                                                                             $500.00</t>
+  </si>
+  <si>
+    <t>Data\Input\02-Short-stories.pdf</t>
+  </si>
+  <si>
+    <t>Gift Of the Magi_x000D_
+ONE DOLLAR AND EIGHTY-SEVEN cp.vrs. That was all. And sixty_x000D_
+cents of it was in pennies. pennies saved one and two at a time by_x000D_
+bulldozing the grcx•cr and the vegetable man and the butcher_x000D_
+until one's cheek burned with the silent imputation of parsimony_x000D_
+that such dealing implied. Three times Della counted it._x000D_
+One dollar and eighty—seven Cents. And the next day would be_x000D_
+Christma s._x000D_
+There uas clearly nothing left to do but flop dou•n on the_x000D_
+shabby little couch and howl. So Della did it. Which instigates the_x000D_
+moral reflection that life is made up Of sobs, sniffles, and smiles,_x000D_
+with sniffles predominating._x000D_
+VVhiIe the mistress of the home is gradually subsiding from the_x000D_
+first stage to the second, take a 100k at the home. A furnished flat_x000D_
+at $8 per week. It did not exactly Irggar description, but it cer-_x000D_
+tainly had that word on the lcnjk•out for the mendicancy squad._x000D_
+In the vestibule Was a into Which no letter_x000D_
+would go, and an electric button from which no mortal finger_x000D_
+cuuld coax a ring. Also aplYrtaining thereunto was a card bearing_x000D_
+the name 'Mr. James Dillingham Young.'_x000D_
+The 'Dillingham' had been flung to the breeze during a former_x000D_
+Of prosperity when its Eumssessor was being paid SS()_x000D_
+week. Now, when incorne was shrunk to $20, the letters of_x000D_
+looked blurred, as though they Were thinking seri-_x000D_
+ously of contracting to a modest and unassuming D. But whenever_x000D_
+Mr. James Dillingham Young came home and reached his flat_x000D_
+above he was called "Jim' and greatly hugged by Mrs. James_x000D_
+Dillingham Young, already introduced to you as Della. Which is_x000D_
+all very_x000D_
+Della finished her cry and attended to her cheeks with the_x000D_
+rag. She by the Window and out dully at a_x000D_
+grey eat walking a grey fence in a grey backyard. To-morrow_x000D_
+would be Christmas Day, and she had only $1.87 with which to_x000D_
+buy Jim a present. She had been saving every penny she could for</t>
+  </si>
+  <si>
     <t>The Gift of the Magi_x000D_
 ONE DOLLAR AND EIGHTY-SEVEN CENTS. That was all. And sixty_x000D_
 cents of it was in pennies. Pennies saved one and two at a time by_x000D_
@@ -315,6 +244,117 @@
 grey cat walking a grey fence in a grey backyard. To-morrow_x000D_
 would be Christmas Day, and she had only $1.87 with which to_x000D_
 buy Jim a present. She had been saving every penny she could for</t>
+  </si>
+  <si>
+    <t>I_x000D_
+The Gift of the Magi_x000D_
+ONE DOLLAR AND EIGH'I'Y-SEVEN CENTS. That was all. And sixty_x000D_
+cents of it was in pennies. Pennies saved one and two at a time by_x000D_
+bulldozing the grocer and the vegetable man and the butcher_x000D_
+until one’s cheek burned with the silent imputation of parsimony_x000D_
+that such close dealing implied. Three times Della counted it._x000D_
+One dollar and eighty-seven cents. And the next day would be_x000D_
+Christmas._x000D_
+There was clearly nothing left to do but flop down on the_x000D_
+' shabby little couch and bowl. So Della did it. Which instigates the_x000D_
+moral reﬂection that life is made up of sobs, snifﬂes, and smiles,_x000D_
+with snifﬂes predominating._x000D_
+While the mistress of the home is gradually subsiding from the_x000D_
+ﬁrst stage to the second, take a look at the home. A furnished ﬂat_x000D_
+at $8 per week. It did not exactly beggar description, but it cer-_x000D_
+tainly had that word on the look-out for the mendicancy squad._x000D_
+In the vestibule below was a letter-box into which no letter_x000D_
+would go, and an electric button from which no mortal ﬁnger_x000D_
+could coax a ring. Also appertaining thereunto was a card bearing_x000D_
+the name ‘Mr. James Dillingham Young.’_x000D_
+The ‘Dillingham’ had been ﬂung to the breeze during a former_x000D_
+period of prosperity when its possessor was being paid $30 per_x000D_
+week. Now, when the income was shrunk to $20, the letters of_x000D_
+‘Dillingham’ looked blurred, as though they were thinking seri-_x000D_
+ously of contracting to a modest and unassuming D. But whenever_x000D_
+Mr. James Dillingham Young came home and reached his ﬂat_x000D_
+above he was called ‘Jim’ and greatly hugged by Mrs. James_x000D_
+Dillingham Young, already introduced to you as Della. Which is_x000D_
+all very good._x000D_
+Della ﬁnished her cry and attended to her cheeks with the_x000D_
+powder rag. She stood by the window and looked out dully at a_x000D_
+grey cat walking a grey fence in a grey backyard. To-morrow_x000D_
+would be Christmas Day, and she had only $1.87 with which to_x000D_
+buy Jim 3 present. She had been saving every penny she could for</t>
+  </si>
+  <si>
+    <t>﻿                       I_x000D_
+ Vhe Gift of the Magi_x000D_
+One dollar and eighty-seven cents. That was all. And sixty_x000D_
+cents of it was in pennies. Pennies saved one and two at a time by_x000D_
+bulldozing the grocer and the vegetable man and the butcher_x000D_
+until one’s cheek burned with the silent imputation of parsimony_x000D_
+that such close dealing implied. Three times Della counted it._x000D_
+One dollar and eighty-seven cents. And the next day would be_x000D_
+Christmas._x000D_
+There was clearly nothing left to do but flop down on the_x000D_
+shabby little couch and howl. So Della did it. Which instigates the_x000D_
+moral reflection that life is made up of sobs, sniffles, and smiles,_x000D_
+with sniffles predominating._x000D_
+While the mistress of the home is gradually subsiding from the_x000D_
+first stage to the second, take a look at the home. A furnished flat_x000D_
+at $8 per week. It did not exactly beggar description, but it cer-_x000D_
+tainly had that word on the look-out for the mendicancy squad._x000D_
+In the vestibule below was a letter-box into which no letter_x000D_
+would go, and an electric button from which                      no mortal finger_x000D_
+could coax a ring. Also appertaining thereunto            was a card bearing_x000D_
+the name ‘Mr. James Dillingham Young.’_x000D_
+The ‘Dillingham’ had been flung to the hreeze during a former_x000D_
+period of prosperity when its possessor was being paid $30 per_x000D_
+week. Now, when the income was shrunk to $20, the letters of_x000D_
+‘Dillingham’ looked blurred, as though they were thinking seri-_x000D_
+ously of contracting to a modest and unassuming D. But whenever_x000D_
+Mr. James Dillingham Young came home and reached his flat_x000D_
+above he was called ‘Jim’ and greatly hugged by Mrs. James_x000D_
+Dillingham Young, already introduced to you as Della. Which is_x000D_
+all very good._x000D_
+Della finished her cry and attended to her cheeks with the_x000D_
+powder rag. She stood by the window and looked out dully at a_x000D_
+grey cat walking a grey fence in a grey backyard. To-morrow_x000D_
+would be Christmas Day, and she had only $1.87 with which to_x000D_
+buy Jim a present. She had been saving every penny she could for</t>
+  </si>
+  <si>
+    <t>Data\Input\03-Invoice-sample.pdf</t>
+  </si>
+  <si>
+    <t>C gtirpd/nroirm_x000D_
+From:_x000D_
+DEMO - Sliced Invoices_x000D_
+suite SA.1204_x000D_
+123 Somewhere Street_x000D_
+Your City AZ 12345_x000D_
+admin Com_x000D_
+Test Business_x000D_
+123 Somewhere St_x000D_
+Melbourne. VIC 3000_x000D_
+test@test.com Invoice Number_x000D_
+Order Number_x000D_
+Invoice Date_x000D_
+Oue Oate_x000D_
+Total Due_x000D_
+RaWPrice_x000D_
+Sas co Sub Total_x000D_
+Total Invoice_x000D_
+INV-3337_x000D_
+January 25, 2016_x000D_
+January 31 2016_x000D_
+Hrs/Qty_x000D_
+1.00_x000D_
+ANZ Bank Service_x000D_
+Web Design_x000D_
+This is a sample description... Adjust Sub Total_x000D_
+$85.00_x000D_
+ACCS 1234 1234_x000D_
+4321 432_x000D_
+Payment is due within 30 days from date of invoice. Late payment is subject to fees of per month._x000D_
+Thanks for choosing DEMO - Sliced Invoices admin@slicedinvoices.com_x000D_
+Page III</t>
   </si>
   <si>
     <t>SlicedInvoices_x000D_
@@ -365,6 +405,282 @@
 Thanks for choosing DEMO - Sliced Invoices | admin@slicedinvoices.com_x000D_
 Page 1/1</t>
   </si>
+  <si>
+    <t>Qgé’é'ced/xzi/oiceo_x000D_
+From I Invoice Number I le-3337 I_x000D_
+DEMO - Sliced Invoices I Order Number I 12345 I_x000D_
+Suite 5A-1204 I invoice Date I January 25, 2016 I_x000D_
+123 Somewhere Street I Due Date I January 31, 2016 I_x000D_
+Your City AZ 12345_x000D_
+admin@s|icedinvoices.com I Total Due I $9350 I_x000D_
+To:_x000D_
+Test Business_x000D_
+123 Somewhere St_x000D_
+Melbourne, VIC 3000 ,_x000D_
+test@test.com -_x000D_
+I Hrs/Qty I Service , I , I Rate/Price I Adjust I Sub Total I_x000D_
+Web Design , 77 7_x000D_
+I 1'00 I This is a sample description... I $8500 I (100% I $8500 I_x000D_
+I . Sub Total I $85.00 I_x000D_
+. ‘ ' I Tax I $8.50 I_x000D_
+I Total I $93.50 I_x000D_
+ANZ Bank_x000D_
+ACC # 1234 1234 ,_x000D_
+BSB # 4321 432 ._x000D_
+Payment is due within 30 days from date of invoice. Late payment is subject to fees of 5% per month._x000D_
+Thanks for choosing DEMO - Sliced Invoices l admin@s|icedinvoices.com_x000D_
+Page 1/1</t>
+  </si>
+  <si>
+    <t>﻿                                    S(iiaed/n)/oi£e&amp;,_x000D_
+                                                                                                                                                         Invoice_x000D_
+                                                                                            Invoice Number                                 INV-3337_x000D_
+From:_x000D_
+DEMO - Sliced Invoices                                                                      Order Number                                   12345_x000D_
+Suite 5A-1204                                                                               Invoice Date                                   January 25, 2016_x000D_
+123 Somewhere Street_x000D_
+                                                                                            Due Date                                       January 31,2016_x000D_
+Your City AZ 12345_x000D_
+admin@slicedinvoices.com                                                                    Total Due                                      S93.50_x000D_
+To:_x000D_
+Test Business_x000D_
+123 Somewhere St_x000D_
+Melbourne, VIC 3000_x000D_
+test@test.com_x000D_
+ Hrs/Qty                                           Service                                  Rate/Price                                Adjust                  Sub Total_x000D_
+                               1.00                Web Design                                   $85.00                                 0.00%                    $85.00_x000D_
+                                                   This is a sample description..._x000D_
+                                                                                                              Sub Total                                         $85.00_x000D_
+                                                                                                                              Tax                                  $8.50_x000D_
+                                                                                                                          Total                                 $93.50_x000D_
+ANZ Bank_x000D_
+ACC # 1234 1234_x000D_
+BSB # 4321 432_x000D_
+Payment is due within 30 days from date of invoice. Late payment is subject to fees of 5% per month._x000D_
+Thanks for choosing DEMO - Sliced Invoices I admin@slicedinvoices.com_x000D_
+Page 1/1</t>
+  </si>
+  <si>
+    <t>Data\Input\04-Scanned-Invoice-Handwritten.pdf</t>
+  </si>
+  <si>
+    <t>From (Senemhf_x000D_
+To (Receiver)_x000D_
+OR. PATR" PERFORMA INVOICE_x000D_
+INVOICE NO. :_x000D_
+THROUGH #_x000D_
+AWB. NO. #_x000D_
+ORI N INVOICE DATE :_x000D_
+s.N0. DES_x000D_
+PRICE_x000D_
+PER UNIT ATION_x000D_
+TOTAL_x000D_
+PRICE DESCRIPTION OF CONTENTS_x000D_
+mooezs ,_x000D_
+fnooe;s_x000D_
+S HAVE NO COMMERCIAL VALUE. UNITS_x000D_
+VALUE DECLARED IS ONLY FOR CUSTOM PURPOSES._x000D_
+SAMPLES ARE STRICTLY NOT FOR RESALE._x000D_
+AMOUNT IN WORDS : GNATURE</t>
+  </si>
+  <si>
+    <t>PERFORMA INVOICE_x000D_
+From (Sender)_x000D_
+EDR. (NAMAN KAPUR_x000D_
+INVOICE NO. :_x000D_
+INVOICE DATE :_x000D_
+- nous_x000D_
+20/4/13_x000D_
+THROUGH #_x000D_
+AWB. NO. #_x000D_
+To (Receiver)_x000D_
+DR. PATAN RAF ULLA KHAN_x000D_
+ORIGIN_x000D_
+DESTINATION_x000D_
+Della_x000D_
+Hindupur_x000D_
+HINDUPUR - 515 201 ( AP )_x000D_
+S.NO_x000D_
+DESCRIPTION OF CONTENTS_x000D_
+UNITS_x000D_
+PRICE_x000D_
+TOTAL_x000D_
+PER UNIT_x000D_
+PRICE_x000D_
+ACUsuppliEs ITEMS_x000D_
+FACE NEEDLES_x000D_
+JNR_x000D_
+2_x000D_
+BaDy NEEDLES_x000D_
+1000 /2_x000D_
+BODY_x000D_
+MODELS._x000D_
+HEAD_x000D_
+MODES_x000D_
+BFC_x000D_
+2148 82476_x000D_
+SAMPLES HAVE NO COMMERCIAL VALUE._x000D_
+VALUE DECLARED IS ONLY FOR CUSTOM PURPOSES._x000D_
+SAMPLES ARE STRICTLY NOT FOR RESALE_x000D_
+AMOUNT IN WORDS :_x000D_
+ONE thousand only._x000D_
+1000_x000D_
+Theera._x000D_
+SIGNATURE</t>
+  </si>
+  <si>
+    <t>9 9 f 99LERF09RM|N9EIC£ 9 j_x000D_
+FromISeﬁn 'r) “ ' g *: -ilI,Nv0I9ENo~1;i:|INv0ICEDATE9I91 = g_x000D_
+._ '1 Magda}747;“§_.//9669L€z°77 I THRQUG‘H#';'5ff"‘f’f‘;:.g'gﬁ-i-‘ff:9; ._x000D_
+I '_ . 999995997779 99999; 9L9994‘KII99 I AWB.NO. #I-gg. , 9* 1‘ V _ . 3_x000D_
+9 .TO (Receiver) _ ‘ 9 I . - 9:97:19 999 99999 ‘_ 99" 9 9 997 :.1-9 if '_x000D_
+, 193779;; ‘ 1%” 70d!) KW? Li QIB|§JN9 9199 D9E§J.NAIIDN99,J. 7' . ?_x000D_
+~~ W. &gt; a . ' IM I—IImoIIiM9_x000D_
+I i'ngiIIwPIIK4-SI8299W J f 7;. ” j 9; ;_x000D_
+ff*";: *:7 7’ 9 ngW=&gt;=TOTrAL ' _'_x000D_
+9 wwﬂf [EESCRFPTpNg-JFCOPTENTS 99 "UN-'73."..PERUNITl“ PBLCE' ‘ "i ?_x000D_
+. . *gwgmutasmﬁ; - .. , =_x000D_
+:I ‘ FMS"; “mugs ~ '- -- : ET ' ,_x000D_
+I 92993353" ~~@**“‘i’“‘~‘f&lt;‘*‘“f‘*ﬁ“ irgjfi' j' 9‘ 9751‘: i_x000D_
+/ 9 - .._x000D_
+. VPLESH‘AVEVNO‘COMMERCIAL:VALUE.. 9 .T ‘ . ‘ ‘ '_x000D_
+' '~_:|:IALUEDECLAREDISONLYFORCUSTOMPURPOSES. . 9. ‘ - 9 '_x000D_
+I 9 SAM???ARESTR'EILYE‘IFQRR5559“ 9 ' i_x000D_
+» . "AMQITNTMWORDS: 7 .739 7’, . .57" I . 9 -“F/9’099/9cﬂ "_x000D_
+. _ CHE":~9H1'OLLSCTY“)01&gt;’)2‘7=—#”a‘1 ’ 9_x000D_
+, 91‘_x000D_
+.~ 4 . - A 13?_x000D_
+. , . . - .9 9 _ ._ .. - wig-2.5}</t>
+  </si>
+  <si>
+    <t>﻿                                                                                                                                              1_x000D_
+                                                                  PJRFORMA INVOICE_x000D_
+   From (Sender)                                                                          INVOICE NO.:             INVOICE DATE:_x000D_
+   g&gt;^. (WAf                                                                                                          %c[dl3_x000D_
+                                                  I_x000D_
+                                                  I            /lc*W                       THROUGH#_x000D_
+                                                                       ---1■■*_x000D_
+                                                                                           AWB. NO. #_x000D_
+   To (Receiver)_x000D_
+                                         Pmtl OLlfi MH                                            ORIGIN              DESTINATION_x000D_
+   S.NO.                                   DESCRIPTION OF CONTENTS                                      UNITS      PRICE          TOTAL_x000D_
+                                                                                                                   PER UNIT       PRICE_x000D_
+                                                                                       1_x000D_
+    1                                                                                                                       V (erc^_x000D_
+                                                               W*A -                                                                          ♦_x000D_
+                                                               Aiqqes_x000D_
+I_x000D_
+   SAMPLES HAVE NO COMMERCIAL VALUE._x000D_
+   VALUE DECLARED IS ONLY FOR CUSTOM PURPOSES._x000D_
+   ___SAMPLES ARE STRICTLY NOT FOR RESALE._x000D_
+   AMOUNT IN WORDS : 1                                                                                            SIGNATURE_x000D_
+   CNe -4ousaw</t>
+  </si>
+  <si>
+    <t>Data\Input\05-good-hand-written-bill.pdf</t>
+  </si>
+  <si>
+    <t>VISHAL PUNJABI_x000D_
+Rool taste dl PJtvnbi load. India. lain Iocd Voq (hirew_x000D_
+PURE VEGIVARIAN fAMiLY RESTAURANT_x000D_
+HOTEL SUN.N.SUN, BOULEVARD ROAD, C.2. SRINAGAR_x000D_
+No_x000D_
+ant},_x000D_
+Thani vou. Particulars Dated."_x000D_
+Amount p._x000D_
+mota'_x000D_
+%pl. Pzc$.inr:</t>
+  </si>
+  <si>
+    <t>Gopal ._x000D_
+VISHAL PUNJABI VAISHNO BHOJANALYA_x000D_
+Real taste of Punjabi load, South Indian, Worth India, Jain Food, Vog Chinese_x000D_
+PURE VEGETARIAN FAMILY RESTAURANT_x000D_
+HOTEL SUN-N-SUN, BOULEVARD ROAD, G-2, SRINAGAR_x000D_
+18_x000D_
+No_x000D_
+.1687_x000D_
+Dated..29 95. 91.._x000D_
+15_x000D_
+anty._x000D_
+Particulars_x000D_
+Rs._x000D_
+Amount_x000D_
+P_x000D_
+1._x000D_
+Khich with Buller ._x000D_
+35-_x000D_
+Knoya Kaju.._x000D_
+So -_x000D_
+Q. Curd._x000D_
+4. Rate_x000D_
+1. Rice._x000D_
+19-_x000D_
+ast_x000D_
+146 to_x000D_
+Total_x000D_
+146_x000D_
+Thank you._x000D_
+Spl. Arrangement for Packing_x000D_
+Signature</t>
+  </si>
+  <si>
+    <t>‘T'ﬂ—" "",w':—""" V'w' " ' ' '7 ' 7 7 if '7 '7 ’ 7 7'7’ ’— Vi‘ ,, " “‘1’" W"_x000D_
+[ - .~’1'H:‘L_x000D_
+1.3-,é77z77v:=53 :7;:‘ ‘;=#‘uv-b . ' ' ‘ ‘-—* ,, ,, .777::»= ”7777;, , 7,7._x000D_
+r a “H H W! air-HEW W . , r .1: mm_x000D_
+‘~ 15915“!qu ! 113‘; ‘33:} 1 r£‘?~"f}"1.ﬂ‘~':'~=€ 1‘! RQ‘JIJ‘JM! E M_x000D_
+Rnulltaslnul'li‘Ju'M‘Ii,IJ{I'3:.’1;‘"1”"' "m '. 4” " '1' in. lainl'a‘t«3,"\‘m.fhircm_x000D_
+m runE-VEGIIJ§?14,P£.EN~1LLIRgmumu-u 1_x000D_
+l' " .{grztaiiii‘iﬁfél‘lfbllﬂﬂﬁgﬂﬂzl; iTJJLf”;-?‘:,_:3Tﬁiif_x000D_
+I'VE- 3 N07,; 8‘ 8r} , ,,,,,, ; 77 7777:, ché~3ﬁ\&lt;&gt;‘~\m_x000D_
+‘" iﬂ’ ‘ V - 7 . “77:11‘3_x000D_
+PEI [1074' 7 (3:535, o ,: ,,, i1_x000D_
+1 m. :75; 77—7——_ vﬁwv‘f'Wﬁﬁgé v- , 7-, «7577777 77 .77_,7,,,_x000D_
+MC? ﬁ: 77 777 77777 ,,,,,,_:7._—7,__,,7 : 7 777 -77 7 7—_x000D_
+M ' ‘ c l‘ ’ ' 9‘1 1_x000D_
+F 1' K‘ha'ch H. with -.13uul,5~ei7r - 73.37% «7_x000D_
+L377. ‘0 l&lt;hmgt I3 . K31 U! a ﬁg 777 1_x000D_
+50' 03- 27(1er .~ 5311 t_x000D_
+[if “‘ RM? 13 . 7_x000D_
+if? " “ '3“— . - 59f_x000D_
+7’ m, 6. '_x000D_
+i - 1 ’ 7 I. n’_x000D_
+:3 ‘ ., : a_x000D_
+{5" P 1 , _ 1" . 'l_x000D_
+:f'r h" V " 1L161$~71073 I_x000D_
+:3 C‘ II_x000D_
+I_x000D_
+1‘ Total f Hit..._x000D_
+£'~'-‘-~"7;"A—-‘&lt;I'_*7_7N_1_; j !. , _ _p__n_u', , , s ‘ngt: B '—?'7.-1_.::, f:f:\t::;::_—::f</t>
+  </si>
+  <si>
+    <t>﻿            VISHAL PUN JABI vAISHNO BHOJANALYA I_x000D_
+&lt;!| •_x000D_
+            Roni toUc ol Pjnjobi hod, ilH Iniinn. hurtb India                                                                             lood, Vog Chirem I_x000D_
+                                                                          PURE VEGETARIAN FAMILY R                                        ANT_x000D_
+                                                                                        ,BOU                            I            B                       ___                I_x000D_
+1             V_x000D_
+                                                                                                                                              •4•»*_x000D_
+                                                                                        I_x000D_
+MO.                                                                                                                                       Amount_x000D_
+       .1                                                                            Particulars                                        I u._x000D_
+                                                    I T4_x000D_
+ft                                                  7"_x000D_
+                                                          Khi'ehrl uoOh C3&gt;u«J4e&lt; •                                                                 3s-»«-_x000D_
+                                                    v     l&lt;no^ck                                                                          So                        ---•_x000D_
+                                                    c9.   Curd*_x000D_
+                                                          Rafi’                                                                                       15-f_x000D_
+                                                          •’ I                                                                             ---^-r  ;_x000D_
+                                                          Kite,_x000D_
+       i_x000D_
+                                                                                                                                                  146_x000D_
+                                                                                        I J                     I_x000D_
+                                                                                                                                                        I_x000D_
+                                                                                                                             Total              Stgntfur*_x000D_
+           Thwii you._x000D_
+       *- ■</t>
+  </si>
 </sst>
 </file>
 
@@ -387,7 +703,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -395,32 +711,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,118 +1033,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46D83C0-E6A1-4EEC-8610-708AB413E818}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725D742F-692F-4424-BACB-5D5EB32E4726}">
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="28" style="1" customWidth="1"/>
-    <col min="3" max="3" width="97.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="270" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="345.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>